<commit_message>
TestNG dataprovider with excel integration added
</commit_message>
<xml_diff>
--- a/DataForDataDrivenTesting.xlsx
+++ b/DataForDataDrivenTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1292398239facc1f/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{FEDD47CD-35D4-4D07-A4EF-A924C34816D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD29F4CA-E770-4137-80BC-09F939F9D9D1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4E38468F-8309-4707-A3A3-D3AC45C2B369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92376BA5-C1CA-4634-BA0A-4BC8CE64E3D6}"/>
   <bookViews>
     <workbookView xWindow="924" yWindow="876" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TestCase</t>
   </si>
@@ -58,9 +58,6 @@
     <t>nk</t>
   </si>
   <si>
-    <t>ksk</t>
-  </si>
-  <si>
     <t>sufis</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t>tea</t>
-  </si>
-  <si>
-    <t>bed</t>
   </si>
   <si>
     <t>book</t>
@@ -141,10 +135,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,7 +403,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,7 +422,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -445,8 +435,8 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -454,13 +444,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -468,13 +458,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -482,13 +472,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>